<commit_message>
Added new values to cost table
</commit_message>
<xml_diff>
--- a/ExcelTables/cost_matrix_pereira_complete.xlsx
+++ b/ExcelTables/cost_matrix_pereira_complete.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanb\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanb\OneDrive\Documentos\GitHub\GerenciaProyectos\ExcelTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4CD012-27C7-4656-ADC7-EC04565AF584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C919D37-4DA4-4F29-A2E6-276CFF1F65A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="140">
   <si>
     <t>Item</t>
   </si>
@@ -452,6 +452,9 @@
   </si>
   <si>
     <t>Normatividad</t>
+  </si>
+  <si>
+    <t>Tipo</t>
   </si>
 </sst>
 </file>
@@ -499,7 +502,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -545,6 +548,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -640,7 +655,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -675,6 +690,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -684,9 +702,20 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -990,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U45"/>
+  <dimension ref="A1:U52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="T57" sqref="T56:T57"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="T44" sqref="T44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3715,7 +3744,7 @@
       <c r="D41" s="9">
         <v>1</v>
       </c>
-      <c r="E41" s="19">
+      <c r="E41" s="16">
         <v>2000000</v>
       </c>
       <c r="F41" s="7">
@@ -3894,60 +3923,60 @@
       </c>
     </row>
     <row r="44" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="16" t="s">
+      <c r="A44" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="B44" s="17"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="18"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="19"/>
       <c r="H44" s="15">
-        <f>SUM(H2:H43)</f>
+        <f t="shared" ref="H44:S44" si="17">SUM(H2:H43)</f>
         <v>161900865</v>
       </c>
       <c r="I44" s="15">
-        <f>SUM(I2:I43)</f>
+        <f t="shared" si="17"/>
         <v>75817925</v>
       </c>
       <c r="J44" s="15">
-        <f>SUM(J2:J43)</f>
+        <f t="shared" si="17"/>
         <v>70858925</v>
       </c>
       <c r="K44" s="15">
-        <f>SUM(K2:K43)</f>
+        <f t="shared" si="17"/>
         <v>70817925</v>
       </c>
       <c r="L44" s="15">
-        <f>SUM(L2:L43)</f>
+        <f t="shared" si="17"/>
         <v>70858925</v>
       </c>
       <c r="M44" s="15">
-        <f>SUM(M2:M43)</f>
+        <f t="shared" si="17"/>
         <v>70817925</v>
       </c>
       <c r="N44" s="15">
-        <f>SUM(N2:N43)</f>
+        <f t="shared" si="17"/>
         <v>40258925</v>
       </c>
       <c r="O44" s="15">
-        <f>SUM(O2:O43)</f>
+        <f t="shared" si="17"/>
         <v>39217925</v>
       </c>
       <c r="P44" s="15">
-        <f>SUM(P2:P43)</f>
+        <f t="shared" si="17"/>
         <v>39258925</v>
       </c>
       <c r="Q44" s="15">
-        <f>SUM(Q2:Q43)</f>
+        <f t="shared" si="17"/>
         <v>39217925</v>
       </c>
       <c r="R44" s="15">
-        <f>SUM(R2:R43)</f>
+        <f t="shared" si="17"/>
         <v>39258925</v>
       </c>
       <c r="S44" s="15">
-        <f>SUM(S2:S43)</f>
+        <f t="shared" si="17"/>
         <v>40217925</v>
       </c>
       <c r="T44" s="14">
@@ -3957,6 +3986,95 @@
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="T45" s="11"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B46" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="C46" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" s="23" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B47" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" s="5">
+        <f>SUMIF($B$2:$B$44, B47, $D$2:$D$44)</f>
+        <v>60</v>
+      </c>
+      <c r="D47" s="5">
+        <f>SUMIF($B$2:$B$44, B47, $F$2:$F$44)</f>
+        <v>43502940</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B48" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C48" s="5">
+        <f t="shared" ref="C48:C52" si="18">SUMIF($B$2:$B$44, B48, $D$2:$D$44)</f>
+        <v>3</v>
+      </c>
+      <c r="D48" s="5">
+        <f t="shared" ref="D48:D52" si="19">SUMIF($B$2:$B$44, B48, $F$2:$F$44)</f>
+        <v>270000</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" s="5">
+        <f t="shared" si="18"/>
+        <v>12</v>
+      </c>
+      <c r="D49" s="5">
+        <f t="shared" si="19"/>
+        <v>19200000</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C50" s="5">
+        <f t="shared" si="18"/>
+        <v>118</v>
+      </c>
+      <c r="D50" s="5">
+        <f t="shared" si="19"/>
+        <v>619135100</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" s="5">
+        <f t="shared" si="18"/>
+        <v>1008</v>
+      </c>
+      <c r="D51" s="5">
+        <f t="shared" si="19"/>
+        <v>45900000</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C52" s="25">
+        <f t="shared" si="18"/>
+        <v>12</v>
+      </c>
+      <c r="D52" s="25">
+        <f t="shared" si="19"/>
+        <v>2400000</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>